<commit_message>
almost done with this project
</commit_message>
<xml_diff>
--- a/DB and Documents/tblQuestion_day1.xlsx
+++ b/DB and Documents/tblQuestion_day1.xlsx
@@ -7483,10 +7483,10 @@
   <dimension ref="A1:DK1066"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F128" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H69" sqref="H69"/>
+      <selection pane="bottomRight" activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.25" customHeight="1"/>
@@ -8215,7 +8215,7 @@
       </c>
       <c r="G16" s="120"/>
       <c r="H16" s="82" t="str">
-        <f t="shared" ref="H15:H22" si="3">B17</f>
+        <f t="shared" ref="H16:H22" si="3">B17</f>
         <v>q1_5</v>
       </c>
       <c r="I16" s="82"/>
@@ -15031,8 +15031,8 @@
         <v>449</v>
       </c>
       <c r="G130" s="7"/>
-      <c r="H130" s="5" t="s">
-        <v>450</v>
+      <c r="H130" s="82" t="s">
+        <v>863</v>
       </c>
       <c r="I130" s="5"/>
       <c r="J130" s="7"/>
@@ -15054,7 +15054,7 @@
       </c>
       <c r="U130" s="16" t="str">
         <f t="shared" si="6"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('129', 'sec06','frmmessage', '','‡mKkb 6t †K¬vwib cwigvc','Section 6. Residual Chlorine Measurement','','q516m','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('129', 'sec06','frmmessage', '','‡mKkb 6t †K¬vwib cwigvc','Section 6. Residual Chlorine Measurement','','q601m','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="131" spans="1:21" s="95" customFormat="1" ht="30">
@@ -15075,8 +15075,8 @@
         <v>453</v>
       </c>
       <c r="G131" s="7"/>
-      <c r="H131" s="5" t="s">
-        <v>454</v>
+      <c r="H131" s="82" t="s">
+        <v>864</v>
       </c>
       <c r="I131" s="5"/>
       <c r="J131" s="7"/>
@@ -15098,7 +15098,7 @@
       </c>
       <c r="U131" s="16" t="str">
         <f t="shared" si="6"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('130', 'q601m','frmmessage', '','†K¬vwib cixÿi c~‡e© D³ evwo Z¨vM Kiæb|','Please leave the compound before conducting the chlorine test.','','q517m','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('130', 'q601m','frmmessage', '','†K¬vwib cixÿi c~‡e© D³ evwo Z¨vM Kiæb|','Please leave the compound before conducting the chlorine test.','','q602m','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="132" spans="1:21" s="95" customFormat="1" ht="59.25">
@@ -27105,7 +27105,7 @@
   <dimension ref="A1:H653"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2:H275"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
project done testing not done
</commit_message>
<xml_diff>
--- a/DB and Documents/tblQuestion_day1.xlsx
+++ b/DB and Documents/tblQuestion_day1.xlsx
@@ -7483,10 +7483,10 @@
   <dimension ref="A1:DK1066"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F128" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H131" sqref="H131"/>
+      <selection pane="bottomRight" activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.25" customHeight="1"/>

</xml_diff>

<commit_message>
partial update on 18th april
</commit_message>
<xml_diff>
--- a/DB and Documents/tblQuestion_day1.xlsx
+++ b/DB and Documents/tblQuestion_day1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-450" windowWidth="13485" windowHeight="11760" tabRatio="409"/>
@@ -21,7 +21,7 @@
     <definedName name="_Toc330979578" localSheetId="0">tbFormMain!#REF!</definedName>
     <definedName name="OLE_LINK1" localSheetId="0">tbFormMain!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -5847,7 +5847,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="53">
     <font>
       <sz val="10"/>
@@ -7059,6 +7059,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -7137,6 +7142,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -7171,6 +7177,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7346,14 +7353,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DK1071"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="U16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V23" sqref="V23"/>
+      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.25" customHeight="1"/>
@@ -9163,7 +9170,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('39', 'q3_0','frmsinglechoice', 'tblMainQues','3.0 Avcwb wK GB Lvbvq nvZ‡avqv cvwbi bgybv †mKmb wU c~iY Ki‡Z Pvb?','3.0 Will you be filing out the hand rinse sampling section in this household?','','q3_1_a','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="41" spans="1:115" ht="58.5">
+    <row r="41" spans="1:115" ht="78">
       <c r="A41" s="67">
         <v>40</v>
       </c>
@@ -11773,7 +11780,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('63', 'q4_0','frmsinglechoice', 'tblMainQues','4.0 Avcwb wK GB Lvbvq Lvevi cvwbi bgybv †mKmb wU c~iY Ki‡Z Pvb?','4.0 Will you be filing out the water sampling section in this household?','','q41m','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="273">
+    <row r="65" spans="1:21" ht="292.5">
       <c r="A65" s="67">
         <v>64</v>
       </c>
@@ -12153,7 +12160,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('72', 'q4_8_1','frmsinglechoice', 'tblMainQues','4.8.1 (ch©‡eÿY) (4.4bs cÖ‡kœi DËi 2 n‡j) msiÿbK…Z cvwbUv ‡X‡K ivLv wQj?','4.8.1 (obs) (if 4.4 is 2) Is the container covered?','','q4_8_2','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="74" spans="1:21" s="172" customFormat="1" ht="33">
+    <row r="74" spans="1:21" s="172" customFormat="1" ht="49.5">
       <c r="A74" s="67">
         <v>73</v>
       </c>
@@ -12323,7 +12330,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('76', 'q4_10','frmsinglechoice', 'tblMainQues','4.10 (hw` 4.4 Gi DËi 2 nq) GB Lvevi cvwb wbivc` Kivi Rb¨ Avcwb †Kvb wKQy K‡i‡Qb wK?','4.10 (if 4.4 is 2) Have you done anything to make this water less cloudy or safer to drink? ','','q414m','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="78">
+    <row r="78" spans="1:21" ht="97.5">
       <c r="A78" s="67">
         <v>77</v>
       </c>
@@ -12408,7 +12415,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('78', 'q4_11Other','frmtext', 'tblMainQues','4.17 Ab¨vb¨ (wbw`©ó K‡i wjLyb)','4.17 Other (specify)','','q4_12','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="58.5">
+    <row r="80" spans="1:21" ht="78">
       <c r="A80" s="67">
         <v>79</v>
       </c>
@@ -12940,7 +12947,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('91', 'q4_19','frmsinglechoice', 'tblMainQues','4.19 (cÖkœ Kiæb/ch©‡eÿY) (hw` 4.18 Gi DËi 1 nq) DËi`vZv Møv‡m cvwb fivi Rb¨ wUDeI‡q‡ji cvwb D‡Ëvj‡b †Kvb AwZwi³ cvwb w`‡qwQj wK?','4.25 (Ask/obs) (if 4.18 is 1) Didthe respondent prime the tubewell prior to retrieving the glass of water?','','q4_21','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="59.25">
+    <row r="93" spans="1:21" ht="60">
       <c r="A93" s="67">
         <v>92</v>
       </c>
@@ -13155,7 +13162,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('96', 'q4_22_other','frmtext', 'tblMainQues','4.22 Ab¨vb¨ (wbw`©ó K‡i wjLyb)','4.22 Other (specify)','','q4_23','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="40.5">
+    <row r="98" spans="1:21" ht="60">
       <c r="A98" s="67">
         <v>97</v>
       </c>
@@ -13536,7 +13543,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('105', 'q5_0','frmsinglechoice', 'tblMainQues','5.0 Avcwb wK GB Lvbvq Lv`¨ bgybv †mKmb wU c~iY Ki‡Z Pvb?','5.0 Will you be filing out the food sampling section in this household?','','q5_1','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="214.5">
+    <row r="107" spans="1:21" ht="234">
       <c r="A107" s="67">
         <v>106</v>
       </c>
@@ -14775,7 +14782,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('134', 'sec06','frmmessage', '','‡mKkb 6t †K¬vwib cwigvc','Section 6. Residual Chlorine Measurement','','q601m','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="136" spans="1:21" ht="30">
+    <row r="136" spans="1:21" ht="39">
       <c r="A136" s="67">
         <v>135</v>
       </c>
@@ -26788,9 +26795,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:T281">
-    <filterColumn colId="1"/>
-    <filterColumn colId="2"/>
-    <filterColumn colId="3"/>
     <sortState ref="A9:V52">
       <sortCondition ref="D1:D86"/>
     </sortState>
@@ -26803,7 +26807,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H665"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -37154,7 +37158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DK143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39556,7 +39560,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="31.5">
+    <row r="23" spans="1:21" ht="47.25">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -40043,7 +40047,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="42">
+    <row r="36" spans="1:21" ht="41.25">
       <c r="A36" s="19">
         <v>33</v>
       </c>
@@ -40509,7 +40513,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="19.5">
+    <row r="48" spans="1:21" ht="27">
       <c r="A48" s="19">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Updated on 4th May 2015
</commit_message>
<xml_diff>
--- a/DB and Documents/tblQuestion_day1.xlsx
+++ b/DB and Documents/tblQuestion_day1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2827" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="1120">
   <si>
     <t>Qdesceng</t>
   </si>
@@ -3464,9 +3464,6 @@
     <t>3.1.a Record whether the respondent has washed her hands at any time before this question since you arrived at the household.</t>
   </si>
   <si>
-    <t>3.1.b Record whether the respondent has washed target child’s hands at any time before this question since you arrived at the household.</t>
-  </si>
-  <si>
     <t>3.1.L D³ Lvbvq Avmvi ci †_‡K GB cÖkœwU Kivi Av‡M ch©šÍ †h‡Kvb mg‡q Avcwb Uv‡M©U wkï‡K nvZ ay‡Z †`‡L‡Qb wK?</t>
   </si>
   <si>
@@ -3489,9 +3486,6 @@
   </si>
   <si>
     <t>sec05</t>
-  </si>
-  <si>
-    <t>hw` Avcbvi wkï (Uv‡M©U wkïi bvg ejyb) GLb cvwb †L‡Z PvBZ Zvn‡j Avcwb wKfv‡e Zv‡K cvwb w`‡Zb `qv K‡i Zv Avgv‡K †`Lvb| [hw` Uv‡M©U wkïwU Lye †ewk †QvU nIqvi Kvi‡b cvwb cvb bv K‡i _v‡K, †m‡ÿ‡Î H Uv‡M©U gv‡qi &lt;3 wkï (hw` &lt;3 eq‡mi wkï bv _v‡K, Zvn‡j Avcbvi &lt;5 eq‡mi wkï) GLb cvwb †L‡Z PvB‡j Zv‡K†hfv‡ecvwb w`‡Zb `qv K‡i Zv Avgv‡K †`Lvb| hw` gv‡qi &lt;3 ev &lt;5 eq‡mi wkï bv _v‡K, Zvn‡j gv‡K wRÁvmv Kiæb, GLb Avcwb cvwb †L‡Z PvB‡j †hfv‡e cvwb wb‡Zb `qv K‡i Zv Avgv‡K †`Lvb| (cÖkœ Kiæb Ges ch©‡eÿb Kiæb)</t>
   </si>
   <si>
     <t>4.1 (obs) Is water for drinking currently available?</t>
@@ -5804,7 +5798,13 @@
     <t>Lvevi Av‡Q wKšZz bgybv msMÖ‡ni Dc‡hvMx bq</t>
   </si>
   <si>
-    <t>If (target childs name) wanted a drink of water right now, could you show me how you would give it to him / her? [If target child is too young to drink water, ask: If your child &lt; 3 years (if not available, then your child &lt;5 years)wanted a drink of water right now, could you show me how you would give it to him / her?]  [If the mother has no children &lt;3 or &lt;5 years, ask:  If you wanted a drink of water right now, could you show me how you would get it?]  Ask the question and observe.</t>
+    <t>3.1.b Record whether the respondent or anyone else has washed target child’s hands at any time before this question since you arrived at the household.</t>
+  </si>
+  <si>
+    <t>If (target childs name) wanted a drink of water right now, could you show me how you would give it to him / her? [If target child is too young to drink water, ask: If your child less than 3 years (if not available, then your child less than 5 years)wanted a drink of water right now, could you show me how you would give it to him / her?]  [If the mother has no children less than 3 or less than 5 years, ask:  If you wanted a drink of water right now, could you show me how you would get it?]  Ask the question and observe.</t>
+  </si>
+  <si>
+    <t>hw` Avcbvi wkï (Uv‡M©U wkïi bvg ejyb) GLb cvwb †L‡Z PvBZ Zvn‡j Avcwb wKfv‡e Zv‡K cvwb w`‡Zb `qv K‡i Zv Avgv‡K †`Lvb| [hw` Uv‡M©U wkïwU Lye †ewk †QvU nIqvi Kvi‡b cvwb cvb bv K‡i _v‡K, †m‡ÿ‡Î H Uv‡M©U gv‡qi 3 eQ‡ii †QvU wkï (hw` 3 eQ‡ii †QvU eq‡mi wkï bv _v‡K, Zvn‡j Avcbvi 5 eQ‡ii †QvU eq‡mi wkï) GLb cvwb †L‡Z PvB‡j Zv‡K†hfv‡ecvwb w`‡Zb `qv K‡i Zv Avgv‡K †`Lvb| hw` gv‡qi 3 ev 5 eQ‡ii †QvU eq‡mi wkï bv _v‡K, Zvn‡j gv‡K wRÁvmv Kiæb, GLb Avcwb cvwb †L‡Z PvB‡j †hfv‡e cvwb wb‡Zb `qv K‡i Zv Avgv‡K †`Lvb| (cÖkœ Kiæb Ges ch©‡eÿb Kiæb)</t>
   </si>
 </sst>
 </file>
@@ -11213,7 +11213,7 @@
   <dimension ref="A1:DK1072"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="T90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="U2" sqref="U2:U140"/>
@@ -11353,7 +11353,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>559</v>
@@ -11362,10 +11362,10 @@
         <v>471</v>
       </c>
       <c r="E3" s="74" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="F3" s="69" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="G3" s="71" t="s">
         <v>476</v>
@@ -11400,7 +11400,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C4" s="230" t="s">
         <v>559</v>
@@ -11409,10 +11409,10 @@
         <v>471</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="F4" s="69" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="G4" s="70"/>
       <c r="H4" s="75" t="str">
@@ -11445,7 +11445,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>82</v>
@@ -11454,10 +11454,10 @@
         <v>471</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="F5" s="69" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="G5" s="70"/>
       <c r="H5" s="75" t="str">
@@ -11490,7 +11490,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="75" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C6" s="150" t="s">
         <v>70</v>
@@ -11499,10 +11499,10 @@
         <v>471</v>
       </c>
       <c r="E6" s="154" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="F6" s="155" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="G6" s="70"/>
       <c r="H6" s="75" t="str">
@@ -11535,7 +11535,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C7" s="150" t="s">
         <v>70</v>
@@ -11544,10 +11544,10 @@
         <v>471</v>
       </c>
       <c r="E7" s="74" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="F7" s="69" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G7" s="70"/>
       <c r="H7" s="75" t="str">
@@ -11580,17 +11580,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="75" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C8" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="55"/>
       <c r="E8" s="74" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="G8" s="150"/>
       <c r="H8" s="55" t="str">
@@ -11623,7 +11623,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="75" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C9" s="55" t="s">
         <v>82</v>
@@ -11632,10 +11632,10 @@
         <v>471</v>
       </c>
       <c r="E9" s="74" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="F9" s="69" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G9" s="150"/>
       <c r="H9" s="55" t="str">
@@ -11675,10 +11675,10 @@
       </c>
       <c r="D10" s="55"/>
       <c r="E10" s="74" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F10" s="69" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="G10" s="150"/>
       <c r="H10" s="55" t="str">
@@ -11711,17 +11711,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C11" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="55"/>
       <c r="E11" s="183" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="F11" s="153" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G11" s="150"/>
       <c r="H11" s="55" t="str">
@@ -11763,10 +11763,10 @@
         <v>471</v>
       </c>
       <c r="E12" s="74" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="F12" s="69" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="G12" s="70"/>
       <c r="H12" s="55" t="str">
@@ -11808,10 +11808,10 @@
         <v>471</v>
       </c>
       <c r="E13" s="156" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="F13" s="69" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="G13" s="70"/>
       <c r="H13" s="55" t="s">
@@ -11843,7 +11843,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="75" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C14" s="150" t="s">
         <v>70</v>
@@ -11852,10 +11852,10 @@
         <v>471</v>
       </c>
       <c r="E14" s="74" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="F14" s="69" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="G14" s="70"/>
       <c r="H14" s="55" t="s">
@@ -11896,10 +11896,10 @@
         <v>471</v>
       </c>
       <c r="E15" s="154" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="F15" s="69" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="G15" s="70"/>
       <c r="H15" s="55" t="str">
@@ -11932,7 +11932,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="55" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C16" s="55" t="s">
         <v>114</v>
@@ -11941,10 +11941,10 @@
         <v>471</v>
       </c>
       <c r="E16" s="74" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="F16" s="69" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="G16" s="70"/>
       <c r="H16" s="55" t="str">
@@ -11986,10 +11986,10 @@
         <v>471</v>
       </c>
       <c r="E17" s="74" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="F17" s="182" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="G17" s="70"/>
       <c r="H17" s="55" t="str">
@@ -12031,10 +12031,10 @@
         <v>471</v>
       </c>
       <c r="E18" s="74" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="F18" s="69" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="G18" s="70"/>
       <c r="H18" s="55" t="str">
@@ -12067,7 +12067,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="75" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C19" s="150" t="s">
         <v>70</v>
@@ -12076,10 +12076,10 @@
         <v>471</v>
       </c>
       <c r="E19" s="74" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="F19" s="69" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="G19" s="70"/>
       <c r="H19" s="55" t="s">
@@ -12120,10 +12120,10 @@
         <v>471</v>
       </c>
       <c r="E20" s="74" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="F20" s="69" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="G20" s="70"/>
       <c r="H20" s="55" t="str">
@@ -12156,17 +12156,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="55" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C21" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="55"/>
       <c r="E21" s="156" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="F21" s="76" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="G21" s="70"/>
       <c r="H21" s="55" t="str">
@@ -12208,10 +12208,10 @@
         <v>471</v>
       </c>
       <c r="E22" s="154" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="F22" s="69" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G22" s="70"/>
       <c r="H22" s="55" t="str">
@@ -12244,7 +12244,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="55" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C23" s="71" t="s">
         <v>110</v>
@@ -12253,10 +12253,10 @@
         <v>471</v>
       </c>
       <c r="E23" s="74" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="F23" s="69" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="G23" s="70"/>
       <c r="H23" s="55" t="str">
@@ -12289,7 +12289,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="55" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C24" s="150" t="s">
         <v>70</v>
@@ -12298,10 +12298,10 @@
         <v>471</v>
       </c>
       <c r="E24" s="74" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F24" s="69" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="G24" s="70"/>
       <c r="H24" s="55" t="str">
@@ -12429,7 +12429,7 @@
       </c>
       <c r="D27" s="55"/>
       <c r="E27" s="154" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="F27" s="69" t="s">
         <v>565</v>
@@ -12564,7 +12564,7 @@
         <v>471</v>
       </c>
       <c r="E30" s="184" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="F30" s="69" t="s">
         <v>481</v>
@@ -12608,7 +12608,7 @@
         <v>471</v>
       </c>
       <c r="E31" s="74" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F31" s="69" t="s">
         <v>482</v>
@@ -12784,10 +12784,10 @@
         <v>471</v>
       </c>
       <c r="E35" s="185" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="F35" s="69" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H35" s="55" t="str">
         <f t="shared" si="3"/>
@@ -12867,7 +12867,7 @@
       </c>
       <c r="D37" s="55"/>
       <c r="E37" s="229" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="F37" s="69" t="s">
         <v>32</v>
@@ -12911,10 +12911,10 @@
         <v>471</v>
       </c>
       <c r="E38" s="186" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="F38" s="155" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="H38" s="75" t="s">
         <v>485</v>
@@ -12952,7 +12952,7 @@
       </c>
       <c r="D39" s="55"/>
       <c r="E39" s="74" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F39" s="78" t="s">
         <v>576</v>
@@ -13040,7 +13040,7 @@
         <v>471</v>
       </c>
       <c r="E41" s="187" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="F41" s="69" t="s">
         <v>584</v>
@@ -13177,10 +13177,10 @@
         <v>471</v>
       </c>
       <c r="E42" s="74" t="s">
-        <v>586</v>
-      </c>
-      <c r="F42" s="69" t="s">
         <v>585</v>
+      </c>
+      <c r="F42" s="202" t="s">
+        <v>1117</v>
       </c>
       <c r="G42" s="71"/>
       <c r="H42" s="55" t="str">
@@ -13203,7 +13203,7 @@
       </c>
       <c r="U42" s="230" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('41', 'q3_1_b','frmsinglechoice', 'tblMainQues','3.1.L D³ Lvbvq Avmvi ci †_‡K GB cÖkœwU Kivi Av‡M ch©šÍ †h‡Kvb mg‡q Avcwb Uv‡M©U wkï‡K nvZ ay‡Z †`‡L‡Qb wK?','3.1.b Record whether the respondent has washed target child’s hands at any time before this question since you arrived at the household.','','q3m','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('41', 'q3_1_b','frmsinglechoice', 'tblMainQues','3.1.L D³ Lvbvq Avmvi ci †_‡K GB cÖkœwU Kivi Av‡M ch©šÍ †h‡Kvb mg‡q Avcwb Uv‡M©U wkï‡K nvZ ay‡Z †`‡L‡Qb wK?','3.1.b Record whether the respondent or anyone else has washed target child’s hands at any time before this question since you arrived at the household.','','q3m','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
       <c r="V42" s="71"/>
       <c r="W42" s="71"/>
@@ -13448,10 +13448,10 @@
         <v>471</v>
       </c>
       <c r="E44" s="193" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="F44" s="192" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="G44" s="71"/>
       <c r="H44" s="55" t="s">
@@ -13582,10 +13582,10 @@
         <v>471</v>
       </c>
       <c r="E45" s="193" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="F45" s="192" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="G45" s="71"/>
       <c r="H45" s="55" t="s">
@@ -13716,10 +13716,10 @@
         <v>471</v>
       </c>
       <c r="E46" s="193" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="F46" s="192" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="G46" s="71"/>
       <c r="H46" s="55" t="s">
@@ -13850,10 +13850,10 @@
         <v>471</v>
       </c>
       <c r="E47" s="193" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="F47" s="192" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="G47" s="71"/>
       <c r="H47" s="55" t="s">
@@ -13984,10 +13984,10 @@
         <v>471</v>
       </c>
       <c r="E48" s="193" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="F48" s="192" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="G48" s="71"/>
       <c r="H48" s="55" t="s">
@@ -14118,14 +14118,14 @@
         <v>471</v>
       </c>
       <c r="E49" s="193" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="F49" s="192" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="G49" s="71"/>
       <c r="H49" s="194" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="I49" s="55"/>
       <c r="J49" s="71"/>
@@ -14243,17 +14243,17 @@
         <v>49</v>
       </c>
       <c r="B50" s="194" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="C50" s="194" t="s">
         <v>47</v>
       </c>
       <c r="D50" s="194"/>
       <c r="E50" s="197" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="F50" s="195" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="G50" s="196"/>
       <c r="H50" s="194" t="s">
@@ -14390,10 +14390,10 @@
         <v>471</v>
       </c>
       <c r="E51" s="199" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="F51" s="198" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="G51" s="71" t="s">
         <v>474</v>
@@ -14528,10 +14528,10 @@
         <v>471</v>
       </c>
       <c r="E52" s="199" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="F52" s="198" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="G52" s="71" t="s">
         <v>474</v>
@@ -14666,10 +14666,10 @@
         <v>471</v>
       </c>
       <c r="E53" s="199" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="F53" s="198" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="G53" s="71" t="s">
         <v>474</v>
@@ -14804,10 +14804,10 @@
         <v>471</v>
       </c>
       <c r="E54" s="199" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="F54" s="198" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G54" s="71" t="s">
         <v>474</v>
@@ -14942,10 +14942,10 @@
         <v>471</v>
       </c>
       <c r="E55" s="199" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="F55" s="198" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="G55" s="71" t="s">
         <v>474</v>
@@ -15080,16 +15080,16 @@
         <v>471</v>
       </c>
       <c r="E56" s="199" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="F56" s="198" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="G56" s="71" t="s">
         <v>474</v>
       </c>
       <c r="H56" s="55" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="I56" s="55"/>
       <c r="J56" s="71"/>
@@ -15209,7 +15209,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="55" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C57" s="55" t="s">
         <v>47</v>
@@ -15352,14 +15352,14 @@
         <v>471</v>
       </c>
       <c r="E58" s="200" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="F58" s="79" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G58" s="71"/>
       <c r="H58" s="55" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="I58" s="55"/>
       <c r="J58" s="71"/>
@@ -15479,17 +15479,17 @@
         <v>58</v>
       </c>
       <c r="B59" s="55" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C59" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D59" s="55"/>
       <c r="E59" s="200" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="F59" s="69" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="G59" s="71"/>
       <c r="H59" s="55" t="s">
@@ -15570,7 +15570,7 @@
         <v>471</v>
       </c>
       <c r="E61" s="201" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="F61" s="69" t="s">
         <v>477</v>
@@ -15612,10 +15612,10 @@
         <v>471</v>
       </c>
       <c r="E62" s="164" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="F62" s="165" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="G62" s="166"/>
       <c r="H62" s="55" t="s">
@@ -15649,7 +15649,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="163" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C63" s="150" t="s">
         <v>70</v>
@@ -15658,10 +15658,10 @@
         <v>471</v>
       </c>
       <c r="E63" s="164" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="F63" s="165" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="G63" s="166"/>
       <c r="H63" s="55" t="s">
@@ -15702,10 +15702,10 @@
       </c>
       <c r="D64" s="55"/>
       <c r="E64" s="82" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F64" s="69" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="G64" s="71"/>
       <c r="H64" s="55" t="str">
@@ -15736,7 +15736,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="55" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C65" s="55" t="s">
         <v>82</v>
@@ -15745,10 +15745,10 @@
         <v>471</v>
       </c>
       <c r="E65" s="82" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F65" s="79" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G65" s="71"/>
       <c r="H65" s="55" t="str">
@@ -15774,7 +15774,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('64', 'q4_0','frmsinglechoice', 'tblMainQues','4.0 Avcwb wK GB Lvbvq Lvevi cvwbi bgybv †mKmb wU c~iY Ki‡Z Pvb?','4.0 Will you be filing out the water sampling section in this household?','','q41m','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="273">
+    <row r="66" spans="1:21" ht="312">
       <c r="A66" s="225">
         <v>65</v>
       </c>
@@ -15786,10 +15786,10 @@
       </c>
       <c r="D66" s="55"/>
       <c r="E66" s="232" t="s">
-        <v>594</v>
+        <v>1119</v>
       </c>
       <c r="F66" s="231" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="G66" s="71"/>
       <c r="H66" s="55" t="s">
@@ -15811,7 +15811,7 @@
       </c>
       <c r="U66" s="230" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('65', 'q41m','frmmessage', '','hw` Avcbvi wkï (Uv‡M©U wkïi bvg ejyb) GLb cvwb †L‡Z PvBZ Zvn‡j Avcwb wKfv‡e Zv‡K cvwb w`‡Zb `qv K‡i Zv Avgv‡K †`Lvb| [hw` Uv‡M©U wkïwU Lye †ewk †QvU nIqvi Kvi‡b cvwb cvb bv K‡i _v‡K, †m‡ÿ‡Î H Uv‡M©U gv‡qi &lt;3 wkï (hw` &lt;3 eq‡mi wkï bv _v‡K, Zvn‡j Avcbvi &lt;5 eq‡mi wkï) GLb cvwb †L‡Z PvB‡j Zv‡K†hfv‡ecvwb w`‡Zb `qv K‡i Zv Avgv‡K †`Lvb| hw` gv‡qi &lt;3 ev &lt;5 eq‡mi wkï bv _v‡K, Zvn‡j gv‡K wRÁvmv Kiæb, GLb Avcwb cvwb †L‡Z PvB‡j †hfv‡e cvwb wb‡Zb `qv K‡i Zv Avgv‡K †`Lvb| (cÖkœ Kiæb Ges ch©‡eÿb Kiæb)','If (target childs name) wanted a drink of water right now, could you show me how you would give it to him / her? [If target child is too young to drink water, ask: If your child &lt; 3 years (if not available, then your child &lt;5 years)wanted a drink of water right now, could you show me how you would give it to him / her?]  [If the mother has no children &lt;3 or &lt;5 years, ask:  If you wanted a drink of water right now, could you show me how you would get it?]  Ask the question and observe.','','q4_1','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('65', 'q41m','frmmessage', '','hw` Avcbvi wkï (Uv‡M©U wkïi bvg ejyb) GLb cvwb †L‡Z PvBZ Zvn‡j Avcwb wKfv‡e Zv‡K cvwb w`‡Zb `qv K‡i Zv Avgv‡K †`Lvb| [hw` Uv‡M©U wkïwU Lye †ewk †QvU nIqvi Kvi‡b cvwb cvb bv K‡i _v‡K, †m‡ÿ‡Î H Uv‡M©U gv‡qi 3 eQ‡ii †QvU wkï (hw` 3 eQ‡ii †QvU eq‡mi wkï bv _v‡K, Zvn‡j Avcbvi 5 eQ‡ii †QvU eq‡mi wkï) GLb cvwb †L‡Z PvB‡j Zv‡K†hfv‡ecvwb w`‡Zb `qv K‡i Zv Avgv‡K †`Lvb| hw` gv‡qi 3 ev 5 eQ‡ii †QvU eq‡mi wkï bv _v‡K, Zvn‡j gv‡K wRÁvmv Kiæb, GLb Avcwb cvwb †L‡Z PvB‡j †hfv‡e cvwb wb‡Zb `qv K‡i Zv Avgv‡K †`Lvb| (cÖkœ Kiæb Ges ch©‡eÿb Kiæb)','If (target childs name) wanted a drink of water right now, could you show me how you would give it to him / her? [If target child is too young to drink water, ask: If your child less than 3 years (if not available, then your child less than 5 years)wanted a drink of water right now, could you show me how you would give it to him / her?]  [If the mother has no children less than 3 or less than 5 years, ask:  If you wanted a drink of water right now, could you show me how you would get it?]  Ask the question and observe.','','q4_1','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="67" spans="1:21" ht="39">
@@ -15828,10 +15828,10 @@
         <v>471</v>
       </c>
       <c r="E67" s="228" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F67" s="69" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="G67" s="71"/>
       <c r="H67" s="55" t="s">
@@ -15870,10 +15870,10 @@
         <v>471</v>
       </c>
       <c r="E68" s="229" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="F68" s="69" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="G68" s="71"/>
       <c r="H68" s="55" t="s">
@@ -15912,10 +15912,10 @@
         <v>471</v>
       </c>
       <c r="E69" s="228" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="F69" s="69" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="G69" s="71"/>
       <c r="H69" s="55" t="s">
@@ -15954,10 +15954,10 @@
         <v>471</v>
       </c>
       <c r="E70" s="80" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F70" s="69" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="G70" s="71"/>
       <c r="H70" s="55" t="s">
@@ -15996,10 +15996,10 @@
         <v>471</v>
       </c>
       <c r="E71" s="201" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="F71" s="69" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="G71" s="71"/>
       <c r="H71" s="55" t="s">
@@ -16038,14 +16038,14 @@
         <v>471</v>
       </c>
       <c r="E72" s="80" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F72" s="202" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="G72" s="71"/>
-      <c r="H72" s="55" t="s">
-        <v>278</v>
+      <c r="H72" s="189" t="s">
+        <v>669</v>
       </c>
       <c r="I72" s="55"/>
       <c r="J72" s="71"/>
@@ -16063,7 +16063,7 @@
       </c>
       <c r="U72" s="230" t="str">
         <f t="shared" si="4"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('71', 'q4_6','frmsinglechoice', 'tblMainQues','4.6 (ch©‡eÿY) Møvm ev cvÎwU‡Z Xvjv cvwbi wfZ‡i Zvi nvZ ev nv‡Zi Av½yj †j‡MwQj?','4.6 (obs) Did her hands touch / contact the drinking water?','','q4_14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('71', 'q4_6','frmsinglechoice', 'tblMainQues','4.6 (ch©‡eÿY) Møvm ev cvÎwU‡Z Xvjv cvwbi wfZ‡i Zvi nvZ ev nv‡Zi Av½yj †j‡MwQj?','4.6 (obs) Did her hands touch / contact the drinking water?','','q4131mm','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="73" spans="1:21" ht="39">
@@ -16080,14 +16080,14 @@
         <v>471</v>
       </c>
       <c r="E73" s="203" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F73" s="69" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="G73" s="71"/>
       <c r="H73" s="163" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="I73" s="55"/>
       <c r="J73" s="71"/>
@@ -16113,7 +16113,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="163" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C74" s="163" t="s">
         <v>82</v>
@@ -16122,14 +16122,14 @@
         <v>471</v>
       </c>
       <c r="E74" s="173" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="F74" s="165" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="G74" s="166"/>
       <c r="H74" s="163" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="I74" s="163"/>
       <c r="J74" s="166"/>
@@ -16159,7 +16159,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="163" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C75" s="163" t="s">
         <v>82</v>
@@ -16168,14 +16168,14 @@
         <v>471</v>
       </c>
       <c r="E75" s="34" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="F75" s="177" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="G75" s="166"/>
       <c r="H75" s="163" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I75" s="163"/>
       <c r="J75" s="166"/>
@@ -16205,7 +16205,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="163" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C76" s="163" t="s">
         <v>82</v>
@@ -16214,10 +16214,10 @@
         <v>471</v>
       </c>
       <c r="E76" s="173" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="F76" s="165" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="G76" s="166"/>
       <c r="H76" s="55" t="s">
@@ -16260,10 +16260,10 @@
         <v>471</v>
       </c>
       <c r="E77" s="80" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F77" s="69" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="G77" s="71"/>
       <c r="H77" s="55" t="s">
@@ -16302,10 +16302,10 @@
         <v>471</v>
       </c>
       <c r="E78" s="80" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="F78" s="69" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="H78" s="218" t="s">
         <v>266</v>
@@ -16338,10 +16338,10 @@
         <v>471</v>
       </c>
       <c r="E79" s="74" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="F79" s="69" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="G79" s="150"/>
       <c r="H79" s="55" t="s">
@@ -16369,7 +16369,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="75" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C80" s="150" t="s">
         <v>70</v>
@@ -16413,7 +16413,7 @@
       <c r="A81" s="225">
         <v>80</v>
       </c>
-      <c r="B81" s="55" t="s">
+      <c r="B81" s="189" t="s">
         <v>270</v>
       </c>
       <c r="C81" s="55" t="s">
@@ -16423,15 +16423,14 @@
         <v>471</v>
       </c>
       <c r="E81" s="74" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="F81" s="69" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="G81" s="71"/>
-      <c r="H81" s="55" t="str">
-        <f t="shared" ref="H81:H90" si="5">B82</f>
-        <v>q4131mm</v>
+      <c r="H81" s="75" t="s">
+        <v>670</v>
       </c>
       <c r="I81" s="55"/>
       <c r="J81" s="71"/>
@@ -16447,7 +16446,7 @@
       </c>
       <c r="U81" s="230" t="str">
         <f t="shared" si="4"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('80', 'q4_12','frmyeartomin', 'tblMainQues','4.12 (hw` 4.10Gi DËi 1=n¨vu nq)  AvbygvwbK KZÿb Av‡M Avcwb GB Lvevi cvwb wbivc` K‡i‡Qb? (99=Rvwb bv)','4.12 (if 4.10 is 1)Approximately how long ago did you treat the water? (99=DK)','','q4131mm','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('80', 'q4_12','frmyeartomin', 'tblMainQues','4.12 (hw` 4.10Gi DËi 1=n¨vu nq)  AvbygvwbK KZÿb Av‡M Avcwb GB Lvevi cvwb wbivc` K‡i‡Qb? (99=Rvwb bv)','4.12 (if 4.10 is 1)Approximately how long ago did you treat the water? (99=DK)','','q4132mm','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="82" spans="1:21" ht="58.5">
@@ -16455,7 +16454,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="75" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C82" s="71" t="s">
         <v>47</v>
@@ -16468,9 +16467,8 @@
         <v>480</v>
       </c>
       <c r="G82" s="71"/>
-      <c r="H82" s="75" t="str">
-        <f t="shared" si="5"/>
-        <v>q4132mm</v>
+      <c r="H82" s="75" t="s">
+        <v>274</v>
       </c>
       <c r="I82" s="55"/>
       <c r="J82" s="71"/>
@@ -16486,7 +16484,7 @@
       </c>
       <c r="U82" s="230" t="str">
         <f t="shared" si="4"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('81', 'q4131mm','frmmessage', '','`qv K‡i  DËi`vZvi †`Iqv LvIqvi cvwb cixÿvi Rb¨ bgybv wnmv‡e  ûBj c¨vK e¨v‡M msMÖn Kiæb|','Please collect a drinking water sample by pouring the water from the glass provided by the participant.','','q4132mm','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('81', 'q4131mm','frmmessage', '','`qv K‡i  DËi`vZvi †`Iqv LvIqvi cvwb cixÿvi Rb¨ bgybv wnmv‡e  ûBj c¨vK e¨v‡M msMÖn Kiæb|','Please collect a drinking water sample by pouring the water from the glass provided by the participant.','','q4_13','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="83" spans="1:21" ht="61.5">
@@ -16494,21 +16492,21 @@
         <v>82</v>
       </c>
       <c r="B83" s="75" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C83" s="71" t="s">
         <v>47</v>
       </c>
       <c r="D83" s="55"/>
       <c r="E83" s="204" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="F83" s="79" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="G83" s="71"/>
       <c r="H83" s="75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H81:H90" si="5">B84</f>
         <v>q4_13</v>
       </c>
       <c r="I83" s="55"/>
@@ -16544,10 +16542,10 @@
         <v>471</v>
       </c>
       <c r="E84" s="74" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="F84" s="69" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="G84" s="71"/>
       <c r="H84" s="55" t="str">
@@ -16576,17 +16574,17 @@
         <v>84</v>
       </c>
       <c r="B85" s="75" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C85" s="71" t="s">
         <v>47</v>
       </c>
       <c r="D85" s="55"/>
       <c r="E85" s="205" t="s">
-        <v>1070</v>
-      </c>
-      <c r="F85" s="69" t="s">
-        <v>664</v>
+        <v>1068</v>
+      </c>
+      <c r="F85" s="202" t="s">
+        <v>662</v>
       </c>
       <c r="G85" s="71"/>
       <c r="H85" s="75" t="str">
@@ -16624,10 +16622,10 @@
         <v>471</v>
       </c>
       <c r="E86" s="74" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="F86" s="69" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G86" s="71"/>
       <c r="H86" s="75" t="str">
@@ -16665,10 +16663,10 @@
         <v>471</v>
       </c>
       <c r="E87" s="74" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F87" s="69" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="G87" s="71"/>
       <c r="H87" s="55" t="str">
@@ -16699,17 +16697,17 @@
         <v>87</v>
       </c>
       <c r="B88" s="71" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C88" s="71" t="s">
         <v>47</v>
       </c>
       <c r="D88" s="55"/>
       <c r="E88" s="74" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="F88" s="69" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="G88" s="71"/>
       <c r="H88" s="75" t="str">
@@ -16749,10 +16747,10 @@
         <v>471</v>
       </c>
       <c r="E89" s="74" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="F89" s="69" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="G89" s="71"/>
       <c r="H89" s="75" t="str">
@@ -16790,10 +16788,10 @@
         <v>471</v>
       </c>
       <c r="E90" s="81" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="F90" s="69" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="G90" s="71"/>
       <c r="H90" s="55" t="str">
@@ -16833,13 +16831,13 @@
         <v>471</v>
       </c>
       <c r="E91" s="81" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="F91" s="69" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="H91" s="75" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="R91" s="226" t="s">
         <v>20</v>
@@ -16860,7 +16858,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="75" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C92" s="150" t="s">
         <v>70</v>
@@ -16869,14 +16867,14 @@
         <v>471</v>
       </c>
       <c r="E92" s="74" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="F92" s="69" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G92" s="150"/>
       <c r="H92" s="75" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I92" s="55"/>
       <c r="L92" s="72"/>
@@ -16913,10 +16911,10 @@
         <v>471</v>
       </c>
       <c r="E93" s="74" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="F93" s="69" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="G93" s="71"/>
       <c r="H93" s="75" t="s">
@@ -16955,10 +16953,10 @@
         <v>471</v>
       </c>
       <c r="E94" s="74" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="F94" s="69" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G94" s="71"/>
       <c r="H94" s="75" t="s">
@@ -16988,7 +16986,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="75" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C95" s="150" t="s">
         <v>70</v>
@@ -16997,10 +16995,10 @@
         <v>471</v>
       </c>
       <c r="E95" s="74" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="F95" s="69" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="G95" s="150"/>
       <c r="H95" s="75" t="s">
@@ -17041,10 +17039,10 @@
         <v>471</v>
       </c>
       <c r="E96" s="74" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="F96" s="69" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G96" s="71"/>
       <c r="H96" s="75" t="str">
@@ -17084,10 +17082,10 @@
         <v>471</v>
       </c>
       <c r="E97" s="74" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="F97" s="69" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G97" s="71"/>
       <c r="H97" s="75" t="str">
@@ -17116,7 +17114,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="75" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C98" s="150" t="s">
         <v>70</v>
@@ -17125,10 +17123,10 @@
         <v>471</v>
       </c>
       <c r="E98" s="74" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="F98" s="69" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G98" s="150"/>
       <c r="H98" s="75" t="str">
@@ -17170,10 +17168,10 @@
         <v>471</v>
       </c>
       <c r="E99" s="74" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="F99" s="69" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G99" s="71"/>
       <c r="H99" s="75" t="s">
@@ -17212,10 +17210,10 @@
         <v>471</v>
       </c>
       <c r="E100" s="82" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="F100" s="69" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G100" s="71"/>
       <c r="H100" s="55" t="str">
@@ -17253,10 +17251,10 @@
         <v>471</v>
       </c>
       <c r="E101" s="83" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="F101" s="69" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="G101" s="71"/>
       <c r="H101" s="55" t="str">
@@ -17296,10 +17294,10 @@
         <v>471</v>
       </c>
       <c r="E102" s="74" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="F102" s="69" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="G102" s="71"/>
       <c r="H102" s="75" t="s">
@@ -17338,10 +17336,10 @@
         <v>471</v>
       </c>
       <c r="E103" s="83" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="F103" s="69" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="G103" s="71"/>
       <c r="H103" s="55" t="str">
@@ -17381,10 +17379,10 @@
         <v>471</v>
       </c>
       <c r="E104" s="74" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F104" s="69" t="s">
         <v>1009</v>
-      </c>
-      <c r="F104" s="69" t="s">
-        <v>1011</v>
       </c>
       <c r="G104" s="71"/>
       <c r="H104" s="55" t="str">
@@ -17424,10 +17422,10 @@
         <v>471</v>
       </c>
       <c r="E105" s="74" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F105" s="69" t="s">
         <v>1010</v>
-      </c>
-      <c r="F105" s="69" t="s">
-        <v>1012</v>
       </c>
       <c r="G105" s="71"/>
       <c r="H105" s="55" t="str">
@@ -17458,17 +17456,17 @@
         <v>105</v>
       </c>
       <c r="B106" s="75" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C106" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D106" s="55"/>
       <c r="E106" s="74" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="F106" s="69" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="G106" s="71"/>
       <c r="H106" s="55" t="str">
@@ -17499,7 +17497,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="55" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C107" s="55" t="s">
         <v>82</v>
@@ -17508,10 +17506,10 @@
         <v>471</v>
       </c>
       <c r="E107" s="74" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F107" s="69" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="G107" s="71"/>
       <c r="H107" s="55" t="str">
@@ -17551,10 +17549,10 @@
         <v>471</v>
       </c>
       <c r="E108" s="74" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F108" s="69" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G108" s="71"/>
       <c r="H108" s="55" t="str">
@@ -17594,10 +17592,10 @@
         <v>471</v>
       </c>
       <c r="E109" s="74" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="F109" s="69" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="G109" s="71"/>
       <c r="H109" s="55" t="str">
@@ -17637,10 +17635,10 @@
         <v>471</v>
       </c>
       <c r="E110" s="74" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="F110" s="69" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="G110" s="71"/>
       <c r="H110" s="55" t="str">
@@ -17671,17 +17669,17 @@
         <v>110</v>
       </c>
       <c r="B111" s="55" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C111" s="71" t="s">
         <v>47</v>
       </c>
       <c r="D111" s="55"/>
       <c r="E111" s="74" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="F111" s="69" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G111" s="71"/>
       <c r="H111" s="55" t="str">
@@ -17721,10 +17719,10 @@
         <v>471</v>
       </c>
       <c r="E112" s="74" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="F112" s="69" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G112" s="71"/>
       <c r="H112" s="55" t="str">
@@ -17764,10 +17762,10 @@
         <v>471</v>
       </c>
       <c r="E113" s="74" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="F113" s="69" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G113" s="71"/>
       <c r="H113" s="55" t="str">
@@ -17798,7 +17796,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="55" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C114" s="55" t="s">
         <v>82</v>
@@ -17807,10 +17805,10 @@
         <v>471</v>
       </c>
       <c r="E114" s="74" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="F114" s="69" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="G114" s="71"/>
       <c r="H114" s="55" t="str">
@@ -17841,7 +17839,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="55" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C115" s="55" t="s">
         <v>82</v>
@@ -17850,10 +17848,10 @@
         <v>471</v>
       </c>
       <c r="E115" s="74" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="F115" s="69" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="G115" s="71"/>
       <c r="H115" s="55" t="str">
@@ -17884,7 +17882,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="55" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C116" s="55" t="s">
         <v>82</v>
@@ -17893,10 +17891,10 @@
         <v>471</v>
       </c>
       <c r="E116" s="74" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="F116" s="69" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="G116" s="71"/>
       <c r="H116" s="55" t="str">
@@ -17927,7 +17925,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="55" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C117" s="55" t="s">
         <v>82</v>
@@ -17936,10 +17934,10 @@
         <v>471</v>
       </c>
       <c r="E117" s="74" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="F117" s="69" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G117" s="71"/>
       <c r="H117" s="55" t="str">
@@ -17979,10 +17977,10 @@
         <v>471</v>
       </c>
       <c r="E118" s="74" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F118" s="69" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="G118" s="71"/>
       <c r="H118" s="55" t="str">
@@ -18022,10 +18020,10 @@
         <v>471</v>
       </c>
       <c r="E119" s="207" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="F119" s="206" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="G119" s="71"/>
       <c r="H119" s="55" t="str">
@@ -18065,10 +18063,10 @@
         <v>471</v>
       </c>
       <c r="E120" s="74" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="F120" s="69" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="G120" s="71"/>
       <c r="H120" s="55" t="str">
@@ -18108,10 +18106,10 @@
         <v>471</v>
       </c>
       <c r="E121" s="74" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="F121" s="69" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="G121" s="71"/>
       <c r="H121" s="55" t="str">
@@ -18142,7 +18140,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="55" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C122" s="55" t="s">
         <v>82</v>
@@ -18151,10 +18149,10 @@
         <v>471</v>
       </c>
       <c r="E122" s="74" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="F122" s="69" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="G122" s="71"/>
       <c r="H122" s="55" t="str">
@@ -18185,7 +18183,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="55" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C123" s="55" t="s">
         <v>82</v>
@@ -18194,10 +18192,10 @@
         <v>471</v>
       </c>
       <c r="E123" s="74" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F123" s="69" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="G123" s="71"/>
       <c r="H123" s="55" t="str">
@@ -18228,7 +18226,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="55" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C124" s="55" t="s">
         <v>82</v>
@@ -18237,10 +18235,10 @@
         <v>471</v>
       </c>
       <c r="E124" s="74" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="F124" s="69" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="G124" s="71"/>
       <c r="H124" s="55" t="str">
@@ -18280,10 +18278,10 @@
         <v>471</v>
       </c>
       <c r="E125" s="74" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="F125" s="69" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="G125" s="71"/>
       <c r="H125" s="55" t="str">
@@ -18323,10 +18321,10 @@
         <v>471</v>
       </c>
       <c r="E126" s="74" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="F126" s="69" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G126" s="71"/>
       <c r="H126" s="55" t="str">
@@ -18357,17 +18355,17 @@
         <v>126</v>
       </c>
       <c r="B127" s="55" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C127" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D127" s="55"/>
       <c r="E127" s="74" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="F127" s="69" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="G127" s="71"/>
       <c r="H127" s="55" t="str">
@@ -18407,10 +18405,10 @@
         <v>471</v>
       </c>
       <c r="E128" s="74" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="F128" s="69" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="G128" s="71"/>
       <c r="H128" s="55" t="str">
@@ -18441,7 +18439,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="163" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C129" s="163" t="s">
         <v>70</v>
@@ -18450,10 +18448,10 @@
         <v>471</v>
       </c>
       <c r="E129" s="164" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="F129" s="165" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="G129" s="166"/>
       <c r="H129" s="163" t="str">
@@ -18488,17 +18486,17 @@
         <v>129</v>
       </c>
       <c r="B130" s="55" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C130" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D130" s="55"/>
       <c r="E130" s="74" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="F130" s="69" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="G130" s="71"/>
       <c r="H130" s="55" t="str">
@@ -18538,10 +18536,10 @@
         <v>471</v>
       </c>
       <c r="E131" s="74" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="F131" s="69" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="G131" s="71"/>
       <c r="H131" s="55" t="str">
@@ -18572,17 +18570,17 @@
         <v>131</v>
       </c>
       <c r="B132" s="55" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C132" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D132" s="55"/>
       <c r="E132" s="74" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="F132" s="69" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="G132" s="71"/>
       <c r="H132" s="55" t="str">
@@ -18613,7 +18611,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="55" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C133" s="55" t="s">
         <v>82</v>
@@ -18622,10 +18620,10 @@
         <v>471</v>
       </c>
       <c r="E133" s="74" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="F133" s="69" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="G133" s="71"/>
       <c r="H133" s="55" t="str">
@@ -18656,7 +18654,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="55" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="C134" s="55" t="s">
         <v>114</v>
@@ -18665,14 +18663,14 @@
         <v>471</v>
       </c>
       <c r="E134" s="74" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="F134" s="69" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="G134" s="71"/>
       <c r="H134" s="55" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="I134" s="55"/>
       <c r="J134" s="71"/>
@@ -18698,7 +18696,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="55" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C135" s="55" t="s">
         <v>82</v>
@@ -18707,10 +18705,10 @@
         <v>471</v>
       </c>
       <c r="E135" s="74" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="F135" s="69" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="G135" s="71"/>
       <c r="H135" s="55" t="str">
@@ -18741,7 +18739,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="55" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C136" s="55" t="s">
         <v>47</v>
@@ -18755,7 +18753,7 @@
       </c>
       <c r="G136" s="71"/>
       <c r="H136" s="55" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="I136" s="55"/>
       <c r="J136" s="71"/>
@@ -18781,7 +18779,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="55" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C137" s="55" t="s">
         <v>47</v>
@@ -18795,7 +18793,7 @@
       </c>
       <c r="G137" s="71"/>
       <c r="H137" s="55" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="I137" s="55"/>
       <c r="J137" s="71"/>
@@ -18821,17 +18819,17 @@
         <v>137</v>
       </c>
       <c r="B138" s="55" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C138" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D138" s="55"/>
       <c r="E138" s="74" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="F138" s="69" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="G138" s="71"/>
       <c r="H138" s="55" t="s">
@@ -18870,10 +18868,10 @@
         <v>471</v>
       </c>
       <c r="E139" s="74" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F139" s="69" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="G139" s="71"/>
       <c r="H139" s="55" t="s">
@@ -18912,10 +18910,10 @@
         <v>471</v>
       </c>
       <c r="E140" s="74" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="F140" s="69" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="G140" s="71"/>
       <c r="H140" s="55" t="s">
@@ -30808,8 +30806,8 @@
   <dimension ref="A1:H665"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H287"/>
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
@@ -30850,7 +30848,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C2" s="144" t="s">
         <v>504</v>
@@ -30873,7 +30871,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C3" s="144" t="s">
         <v>506</v>
@@ -30896,7 +30894,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C4" s="144" t="s">
         <v>508</v>
@@ -30919,7 +30917,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C5" s="144" t="s">
         <v>510</v>
@@ -30942,7 +30940,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C6" s="144" t="s">
         <v>512</v>
@@ -30965,7 +30963,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C7" s="144" t="s">
         <v>514</v>
@@ -30988,7 +30986,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C8" s="144" t="s">
         <v>516</v>
@@ -31011,7 +31009,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C9" s="144" t="s">
         <v>518</v>
@@ -31034,7 +31032,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C10" s="144" t="s">
         <v>520</v>
@@ -31057,7 +31055,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C11" s="144" t="s">
         <v>522</v>
@@ -31080,7 +31078,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C12" s="144" t="s">
         <v>524</v>
@@ -31103,7 +31101,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="75" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C13" s="144" t="s">
         <v>526</v>
@@ -31126,7 +31124,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="75" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C14" s="116" t="s">
         <v>567</v>
@@ -31149,7 +31147,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C15" s="116" t="s">
         <v>568</v>
@@ -31225,10 +31223,10 @@
         <v>60</v>
       </c>
       <c r="C18" s="116" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D18" s="138" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="E18" s="58">
         <v>1</v>
@@ -31248,10 +31246,10 @@
         <v>60</v>
       </c>
       <c r="C19" s="116" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D19" s="138" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="E19" s="58">
         <v>2</v>
@@ -31271,16 +31269,16 @@
         <v>60</v>
       </c>
       <c r="C20" s="116" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D20" s="138" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E20" s="58">
         <v>77</v>
       </c>
       <c r="F20" s="75" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="G20" s="61"/>
       <c r="H20" s="111" t="str">
@@ -31296,10 +31294,10 @@
         <v>51</v>
       </c>
       <c r="C21" s="116" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D21" s="138" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="E21" s="112">
         <v>1</v>
@@ -31319,10 +31317,10 @@
         <v>51</v>
       </c>
       <c r="C22" s="116" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D22" s="138" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="E22" s="112">
         <v>2</v>
@@ -31342,10 +31340,10 @@
         <v>51</v>
       </c>
       <c r="C23" s="116" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D23" s="138" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="E23" s="112">
         <v>3</v>
@@ -31365,10 +31363,10 @@
         <v>51</v>
       </c>
       <c r="C24" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D24" s="138" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E24" s="112">
         <v>99</v>
@@ -31388,10 +31386,10 @@
         <v>56</v>
       </c>
       <c r="C25" s="116" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D25" s="138" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="E25" s="58">
         <v>1</v>
@@ -31411,10 +31409,10 @@
         <v>56</v>
       </c>
       <c r="C26" s="116" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D26" s="138" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="E26" s="58">
         <v>2</v>
@@ -31434,16 +31432,16 @@
         <v>56</v>
       </c>
       <c r="C27" s="116" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D27" s="138" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E27" s="58">
         <v>77</v>
       </c>
       <c r="F27" s="75" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="G27" s="61"/>
       <c r="H27" s="111" t="str">
@@ -31459,10 +31457,10 @@
         <v>56</v>
       </c>
       <c r="C28" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D28" s="138" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E28" s="58">
         <v>99</v>
@@ -31528,10 +31526,10 @@
         <v>68</v>
       </c>
       <c r="C31" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D31" s="138" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E31" s="58">
         <v>99</v>
@@ -31548,13 +31546,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C32" s="116" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="D32" s="138" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="E32" s="58">
         <v>1</v>
@@ -31571,13 +31569,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C33" s="116" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D33" s="138" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="E33" s="58">
         <v>1</v>
@@ -31594,13 +31592,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="75" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C34" s="116" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D34" s="138" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="E34" s="58">
         <v>1</v>
@@ -31617,13 +31615,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="75" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C35" s="116" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D35" s="138" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="E35" s="58">
         <v>1</v>
@@ -31640,13 +31638,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C36" s="116" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D36" s="138" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="E36" s="58">
         <v>1</v>
@@ -31663,19 +31661,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="75" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C37" s="116" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D37" s="138" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E37" s="58">
         <v>1</v>
       </c>
       <c r="F37" s="75" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="G37" s="61"/>
       <c r="H37" s="111" t="str">
@@ -31688,13 +31686,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="75" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C38" s="116" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D38" s="138" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E38" s="58">
         <v>1</v>
@@ -31711,13 +31709,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="75" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C39" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D39" s="138" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E39" s="58">
         <v>1</v>
@@ -31811,7 +31809,7 @@
         <v>530</v>
       </c>
       <c r="D43" s="162" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="E43" s="58">
         <v>2</v>
@@ -32023,10 +32021,10 @@
         <v>582</v>
       </c>
       <c r="C52" s="209" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="D52" s="208" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E52" s="58">
         <v>1</v>
@@ -32046,10 +32044,10 @@
         <v>582</v>
       </c>
       <c r="C53" s="209" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D53" s="208" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="E53" s="58">
         <v>2</v>
@@ -32069,10 +32067,10 @@
         <v>582</v>
       </c>
       <c r="C54" s="209" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D54" s="208" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="E54" s="58">
         <v>3</v>
@@ -32092,10 +32090,10 @@
         <v>582</v>
       </c>
       <c r="C55" s="209" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D55" s="208" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="E55" s="58">
         <v>99</v>
@@ -32115,10 +32113,10 @@
         <v>583</v>
       </c>
       <c r="C56" s="209" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="D56" s="208" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="E56" s="58">
         <v>1</v>
@@ -32138,10 +32136,10 @@
         <v>583</v>
       </c>
       <c r="C57" s="209" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="D57" s="208" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="E57" s="58">
         <v>2</v>
@@ -32161,10 +32159,10 @@
         <v>583</v>
       </c>
       <c r="C58" s="209" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D58" s="208" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="E58" s="58">
         <v>3</v>
@@ -32184,10 +32182,10 @@
         <v>583</v>
       </c>
       <c r="C59" s="209" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D59" s="208" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="E59" s="58">
         <v>99</v>
@@ -33587,7 +33585,7 @@
         <v>548</v>
       </c>
       <c r="C120" s="210" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="D120" s="137" t="s">
         <v>549</v>
@@ -33610,7 +33608,7 @@
         <v>550</v>
       </c>
       <c r="C121" s="210" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="D121" s="137" t="s">
         <v>551</v>
@@ -33633,7 +33631,7 @@
         <v>552</v>
       </c>
       <c r="C122" s="210" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="D122" s="137" t="s">
         <v>553</v>
@@ -33656,7 +33654,7 @@
         <v>554</v>
       </c>
       <c r="C123" s="210" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="D123" s="137" t="s">
         <v>555</v>
@@ -33679,7 +33677,7 @@
         <v>556</v>
       </c>
       <c r="C124" s="210" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="D124" s="137" t="s">
         <v>557</v>
@@ -33702,10 +33700,10 @@
         <v>155</v>
       </c>
       <c r="C125" s="210" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D125" s="213" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="E125" s="114">
         <v>1</v>
@@ -33725,10 +33723,10 @@
         <v>155</v>
       </c>
       <c r="C126" s="211" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D126" s="213" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="E126" s="114">
         <v>2</v>
@@ -33748,10 +33746,10 @@
         <v>155</v>
       </c>
       <c r="C127" s="212" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="D127" s="213" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="E127" s="114">
         <v>3</v>
@@ -33771,7 +33769,7 @@
         <v>155</v>
       </c>
       <c r="C128" s="210" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="D128" s="213" t="s">
         <v>34</v>
@@ -33780,7 +33778,7 @@
         <v>77</v>
       </c>
       <c r="F128" s="163" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="G128" s="61"/>
       <c r="H128" s="111" t="str">
@@ -33793,7 +33791,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="57" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C129" s="144" t="s">
         <v>567</v>
@@ -33816,7 +33814,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="57" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C130" s="144" t="s">
         <v>568</v>
@@ -33828,7 +33826,7 @@
         <v>2</v>
       </c>
       <c r="F130" s="75" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G130" s="61"/>
       <c r="H130" s="111" t="str">
@@ -33876,7 +33874,7 @@
         <v>2</v>
       </c>
       <c r="F132" s="75" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G132" s="61"/>
       <c r="H132" s="111" t="str">
@@ -33938,10 +33936,10 @@
         <v>222</v>
       </c>
       <c r="C135" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D135" s="138" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E135" s="58">
         <v>99</v>
@@ -33961,10 +33959,10 @@
         <v>226</v>
       </c>
       <c r="C136" s="116" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="D136" s="138" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E136" s="114">
         <v>1</v>
@@ -33984,10 +33982,10 @@
         <v>226</v>
       </c>
       <c r="C137" s="116" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D137" s="138" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E137" s="58">
         <v>2</v>
@@ -34007,10 +34005,10 @@
         <v>226</v>
       </c>
       <c r="C138" s="172" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D138" s="45" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E138" s="58">
         <v>3</v>
@@ -34030,10 +34028,10 @@
         <v>226</v>
       </c>
       <c r="C139" s="172" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D139" s="45" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="E139" s="58">
         <v>4</v>
@@ -34053,10 +34051,10 @@
         <v>226</v>
       </c>
       <c r="C140" s="116" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D140" s="138" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E140" s="58">
         <v>5</v>
@@ -34076,10 +34074,10 @@
         <v>226</v>
       </c>
       <c r="C141" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D141" s="138" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E141" s="58">
         <v>99</v>
@@ -34099,10 +34097,10 @@
         <v>230</v>
       </c>
       <c r="C142" s="116" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D142" s="138" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E142" s="114">
         <v>1</v>
@@ -34122,10 +34120,10 @@
         <v>230</v>
       </c>
       <c r="C143" s="116" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D143" s="138" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E143" s="58">
         <v>2</v>
@@ -34145,10 +34143,10 @@
         <v>230</v>
       </c>
       <c r="C144" s="116" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D144" s="138" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E144" s="58">
         <v>3</v>
@@ -34168,10 +34166,10 @@
         <v>230</v>
       </c>
       <c r="C145" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D145" s="138" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E145" s="58">
         <v>99</v>
@@ -34191,10 +34189,10 @@
         <v>238</v>
       </c>
       <c r="C146" s="116" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D146" s="138" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="E146" s="114">
         <v>1</v>
@@ -34214,10 +34212,10 @@
         <v>238</v>
       </c>
       <c r="C147" s="116" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D147" s="138" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E147" s="58">
         <v>2</v>
@@ -34237,10 +34235,10 @@
         <v>238</v>
       </c>
       <c r="C148" s="116" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D148" s="214" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="E148" s="58">
         <v>3</v>
@@ -34260,10 +34258,10 @@
         <v>238</v>
       </c>
       <c r="C149" s="116" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D149" s="138" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E149" s="58">
         <v>4</v>
@@ -34283,10 +34281,10 @@
         <v>238</v>
       </c>
       <c r="C150" s="116" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="D150" s="138" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="E150" s="58">
         <v>5</v>
@@ -34306,10 +34304,10 @@
         <v>238</v>
       </c>
       <c r="C151" s="172" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="D151" s="171" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="E151" s="58">
         <v>6</v>
@@ -34329,10 +34327,10 @@
         <v>238</v>
       </c>
       <c r="C152" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D152" s="138" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E152" s="58">
         <v>99</v>
@@ -34398,10 +34396,10 @@
         <v>242</v>
       </c>
       <c r="C155" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D155" s="138" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E155" s="58">
         <v>99</v>
@@ -34421,10 +34419,10 @@
         <v>246</v>
       </c>
       <c r="C156" s="116" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D156" s="138" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E156" s="114">
         <v>1</v>
@@ -34444,10 +34442,10 @@
         <v>246</v>
       </c>
       <c r="C157" s="116" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D157" s="138" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="E157" s="58">
         <v>2</v>
@@ -34467,10 +34465,10 @@
         <v>246</v>
       </c>
       <c r="C158" s="116" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D158" s="138" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="E158" s="58">
         <v>3</v>
@@ -34490,10 +34488,10 @@
         <v>246</v>
       </c>
       <c r="C159" s="116" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D159" s="138" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E159" s="58">
         <v>4</v>
@@ -34513,10 +34511,10 @@
         <v>246</v>
       </c>
       <c r="C160" s="116" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D160" s="215" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="E160" s="58">
         <v>5</v>
@@ -34536,10 +34534,10 @@
         <v>246</v>
       </c>
       <c r="C161" s="116" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D161" s="215" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="E161" s="58">
         <v>6</v>
@@ -34559,10 +34557,10 @@
         <v>246</v>
       </c>
       <c r="C162" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D162" s="138" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E162" s="58">
         <v>99</v>
@@ -34579,13 +34577,13 @@
         <v>162</v>
       </c>
       <c r="B163" s="57" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C163" s="116" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D163" s="138" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E163" s="114">
         <v>1</v>
@@ -34602,13 +34600,13 @@
         <v>163</v>
       </c>
       <c r="B164" s="57" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C164" s="116" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D164" s="138" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="E164" s="58">
         <v>2</v>
@@ -34627,13 +34625,13 @@
         <v>164</v>
       </c>
       <c r="B165" s="57" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C165" s="116" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D165" s="138" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="E165" s="58">
         <v>3</v>
@@ -34652,13 +34650,13 @@
         <v>165</v>
       </c>
       <c r="B166" s="57" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C166" s="116" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D166" s="138" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E166" s="58">
         <v>99</v>
@@ -34677,13 +34675,13 @@
         <v>166</v>
       </c>
       <c r="B167" s="163" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C167" s="176" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D167" s="217" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="E167" s="58">
         <v>1</v>
@@ -34700,7 +34698,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="163" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C168" s="175" t="s">
         <v>568</v>
@@ -34723,7 +34721,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="163" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C169" s="144" t="s">
         <v>567</v>
@@ -34746,7 +34744,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="163" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C170" s="144" t="s">
         <v>568</v>
@@ -34804,7 +34802,7 @@
         <v>2</v>
       </c>
       <c r="F172" s="219" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G172" s="61"/>
       <c r="H172" s="111" t="str">
@@ -34820,16 +34818,16 @@
         <v>262</v>
       </c>
       <c r="C173" s="116" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D173" s="138" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="E173" s="58">
         <v>99</v>
       </c>
       <c r="F173" s="219" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G173" s="61"/>
       <c r="H173" s="111" t="str">
@@ -34842,13 +34840,13 @@
         <v>173</v>
       </c>
       <c r="B174" s="57" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C174" s="144" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="D174" s="137" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E174" s="114">
         <v>1</v>
@@ -34865,13 +34863,13 @@
         <v>174</v>
       </c>
       <c r="B175" s="57" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C175" s="144" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="D175" s="137" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="E175" s="58">
         <v>1</v>
@@ -34888,13 +34886,13 @@
         <v>175</v>
       </c>
       <c r="B176" s="57" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C176" s="144" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="D176" s="137" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="E176" s="114">
         <v>1</v>
@@ -34911,13 +34909,13 @@
         <v>176</v>
       </c>
       <c r="B177" s="57" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C177" s="144" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="D177" s="137" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="E177" s="58">
         <v>1</v>
@@ -34934,13 +34932,13 @@
         <v>177</v>
       </c>
       <c r="B178" s="57" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C178" s="144" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="D178" s="137" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="E178" s="114">
         <v>1</v>
@@ -34957,13 +34955,13 @@
         <v>178</v>
       </c>
       <c r="B179" s="57" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C179" s="144" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="D179" s="137" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E179" s="58">
         <v>1</v>
@@ -34980,13 +34978,13 @@
         <v>179</v>
       </c>
       <c r="B180" s="57" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C180" s="144" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D180" s="137" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="E180" s="114">
         <v>1</v>
@@ -35003,13 +35001,13 @@
         <v>180</v>
       </c>
       <c r="B181" s="57" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C181" s="144" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="D181" s="137" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E181" s="58">
         <v>1</v>
@@ -35026,13 +35024,13 @@
         <v>181</v>
       </c>
       <c r="B182" s="57" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C182" s="144" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="D182" s="137" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="E182" s="114">
         <v>1</v>
@@ -35049,13 +35047,13 @@
         <v>182</v>
       </c>
       <c r="B183" s="57" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C183" s="144" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="D183" s="137" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E183" s="58">
         <v>1</v>
@@ -35072,13 +35070,13 @@
         <v>183</v>
       </c>
       <c r="B184" s="57" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C184" s="144" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="D184" s="139" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="E184" s="114">
         <v>1</v>
@@ -35095,19 +35093,19 @@
         <v>184</v>
       </c>
       <c r="B185" s="57" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C185" s="144" t="s">
         <v>33</v>
       </c>
       <c r="D185" s="137" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="E185" s="58">
         <v>1</v>
       </c>
       <c r="F185" s="75" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="G185" s="61"/>
       <c r="H185" s="111" t="str">
@@ -35155,7 +35153,7 @@
         <v>2</v>
       </c>
       <c r="F187" s="75" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="G187" s="61"/>
       <c r="H187" s="111" t="str">
@@ -35219,10 +35217,10 @@
         <v>295</v>
       </c>
       <c r="C190" s="144" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="D190" s="137" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E190" s="114">
         <v>1</v>
@@ -35244,10 +35242,10 @@
         <v>295</v>
       </c>
       <c r="C191" s="144" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="D191" s="137" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="E191" s="58">
         <v>2</v>
@@ -35267,10 +35265,10 @@
         <v>295</v>
       </c>
       <c r="C192" s="144" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="D192" s="137" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="E192" s="58">
         <v>3</v>
@@ -35290,10 +35288,10 @@
         <v>295</v>
       </c>
       <c r="C193" s="144" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="D193" s="137" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="E193" s="114">
         <v>4</v>
@@ -35313,10 +35311,10 @@
         <v>295</v>
       </c>
       <c r="C194" s="144" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="D194" s="137" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="E194" s="58">
         <v>5</v>
@@ -35336,10 +35334,10 @@
         <v>295</v>
       </c>
       <c r="C195" s="144" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="D195" s="137" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="E195" s="58">
         <v>6</v>
@@ -35359,10 +35357,10 @@
         <v>295</v>
       </c>
       <c r="C196" s="144" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="D196" s="137" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="E196" s="114">
         <v>7</v>
@@ -35382,10 +35380,10 @@
         <v>295</v>
       </c>
       <c r="C197" s="144" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="D197" s="137" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="E197" s="58">
         <v>8</v>
@@ -35405,10 +35403,10 @@
         <v>295</v>
       </c>
       <c r="C198" s="144" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="D198" s="137" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="E198" s="58">
         <v>9</v>
@@ -35428,10 +35426,10 @@
         <v>295</v>
       </c>
       <c r="C199" s="144" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D199" s="137" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="E199" s="114">
         <v>10</v>
@@ -35451,10 +35449,10 @@
         <v>295</v>
       </c>
       <c r="C200" s="144" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="D200" s="137" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="E200" s="58">
         <v>11</v>
@@ -35477,13 +35475,13 @@
         <v>33</v>
       </c>
       <c r="D201" s="137" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="E201" s="58">
         <v>77</v>
       </c>
       <c r="F201" s="75" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G201" s="61"/>
       <c r="H201" s="111" t="str">
@@ -35499,10 +35497,10 @@
         <v>295</v>
       </c>
       <c r="C202" s="144" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D202" s="137" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E202" s="58">
         <v>99</v>
@@ -35570,10 +35568,10 @@
         <v>299</v>
       </c>
       <c r="C205" s="144" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D205" s="137" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E205" s="114">
         <v>99</v>
@@ -35593,10 +35591,10 @@
         <v>310</v>
       </c>
       <c r="C206" s="222" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="D206" s="221" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="E206" s="114">
         <v>1</v>
@@ -35616,10 +35614,10 @@
         <v>310</v>
       </c>
       <c r="C207" s="222" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="D207" s="221" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="E207" s="58">
         <v>2</v>
@@ -35639,10 +35637,10 @@
         <v>310</v>
       </c>
       <c r="C208" s="222" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="D208" s="221" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="E208" s="114">
         <v>3</v>
@@ -35671,7 +35669,7 @@
         <v>4</v>
       </c>
       <c r="F209" s="75" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="G209" s="61"/>
       <c r="H209" s="111" t="str">
@@ -35687,10 +35685,10 @@
         <v>322</v>
       </c>
       <c r="C210" s="222" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="D210" s="221" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="E210" s="114">
         <v>1</v>
@@ -35710,10 +35708,10 @@
         <v>322</v>
       </c>
       <c r="C211" s="222" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="D211" s="221" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="E211" s="58">
         <v>2</v>
@@ -35733,10 +35731,10 @@
         <v>322</v>
       </c>
       <c r="C212" s="222" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="D212" s="221" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="E212" s="114">
         <v>3</v>
@@ -35756,10 +35754,10 @@
         <v>322</v>
       </c>
       <c r="C213" s="222" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="D213" s="221" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="E213" s="58">
         <v>4</v>
@@ -35779,10 +35777,10 @@
         <v>322</v>
       </c>
       <c r="C214" s="222" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="D214" s="221" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="E214" s="58">
         <v>5</v>
@@ -35811,7 +35809,7 @@
         <v>77</v>
       </c>
       <c r="F215" s="75" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G215" s="61"/>
       <c r="H215" s="111" t="str">
@@ -35827,10 +35825,10 @@
         <v>322</v>
       </c>
       <c r="C216" s="222" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D216" s="221" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E216" s="114">
         <v>99</v>
@@ -35898,10 +35896,10 @@
         <v>330</v>
       </c>
       <c r="C219" s="222" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D219" s="221" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E219" s="58">
         <v>99</v>
@@ -35967,10 +35965,10 @@
         <v>334</v>
       </c>
       <c r="C222" s="222" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D222" s="221" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E222" s="58">
         <v>99</v>
@@ -36036,10 +36034,10 @@
         <v>338</v>
       </c>
       <c r="C225" s="222" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D225" s="221" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E225" s="58">
         <v>99</v>
@@ -36107,10 +36105,10 @@
         <v>342</v>
       </c>
       <c r="C228" s="222" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D228" s="221" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E228" s="58">
         <v>99</v>
@@ -36176,10 +36174,10 @@
         <v>354</v>
       </c>
       <c r="C231" s="222" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D231" s="221" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E231" s="58">
         <v>99</v>
@@ -36196,7 +36194,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="75" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C232" s="116" t="s">
         <v>567</v>
@@ -36219,7 +36217,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="75" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C233" s="116" t="s">
         <v>568</v>
@@ -36231,7 +36229,7 @@
         <v>2</v>
       </c>
       <c r="F233" s="75" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="G233" s="61"/>
       <c r="H233" s="111" t="str">
@@ -36304,7 +36302,7 @@
         <v>1</v>
       </c>
       <c r="F236" s="75" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G236" s="61"/>
       <c r="H236" s="111" t="str">
@@ -36375,7 +36373,7 @@
         <v>2</v>
       </c>
       <c r="F239" s="75" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="G239" s="61"/>
       <c r="H239" s="111" t="str">
@@ -36391,10 +36389,10 @@
         <v>396</v>
       </c>
       <c r="C240" s="116" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D240" s="138" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E240" s="117">
         <v>1</v>
@@ -36414,10 +36412,10 @@
         <v>396</v>
       </c>
       <c r="C241" s="116" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="D241" s="138" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="E241" s="117">
         <v>2</v>
@@ -36437,10 +36435,10 @@
         <v>396</v>
       </c>
       <c r="C242" s="116" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D242" s="138" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E242" s="117">
         <v>3</v>
@@ -36457,13 +36455,13 @@
         <v>242</v>
       </c>
       <c r="B243" s="75" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C243" s="116" t="s">
         <v>528</v>
       </c>
       <c r="D243" s="138" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E243" s="117">
         <v>1</v>
@@ -36480,13 +36478,13 @@
         <v>243</v>
       </c>
       <c r="B244" s="75" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C244" s="116" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D244" s="138" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E244" s="117">
         <v>1</v>
@@ -36503,13 +36501,13 @@
         <v>244</v>
       </c>
       <c r="B245" s="75" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C245" s="116" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="D245" s="138" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="E245" s="117">
         <v>1</v>
@@ -36526,13 +36524,13 @@
         <v>245</v>
       </c>
       <c r="B246" s="75" t="s">
+        <v>785</v>
+      </c>
+      <c r="C246" s="116" t="s">
         <v>787</v>
       </c>
-      <c r="C246" s="116" t="s">
-        <v>789</v>
-      </c>
       <c r="D246" s="138" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="E246" s="117">
         <v>1</v>
@@ -36549,13 +36547,13 @@
         <v>246</v>
       </c>
       <c r="B247" s="118" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C247" s="116" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D247" s="138" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E247" s="117">
         <v>1</v>
@@ -36572,19 +36570,19 @@
         <v>247</v>
       </c>
       <c r="B248" s="119" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C248" s="116" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D248" s="138" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="E248" s="117">
         <v>2</v>
       </c>
       <c r="F248" s="56" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="G248" s="61"/>
       <c r="H248" s="111" t="str">
@@ -36597,19 +36595,19 @@
         <v>248</v>
       </c>
       <c r="B249" s="119" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C249" s="116" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D249" s="138" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E249" s="114">
         <v>3</v>
       </c>
       <c r="F249" s="56" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="G249" s="61"/>
       <c r="H249" s="111" t="str">
@@ -36622,19 +36620,19 @@
         <v>249</v>
       </c>
       <c r="B250" s="119" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C250" s="116" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="D250" s="138" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E250" s="114">
         <v>99</v>
       </c>
       <c r="F250" s="56" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="G250" s="61"/>
       <c r="H250" s="111" t="str">
@@ -36647,13 +36645,13 @@
         <v>250</v>
       </c>
       <c r="B251" s="119" t="s">
+        <v>794</v>
+      </c>
+      <c r="C251" s="116" t="s">
         <v>796</v>
       </c>
-      <c r="C251" s="116" t="s">
-        <v>798</v>
-      </c>
       <c r="D251" s="223" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="E251" s="58">
         <v>1</v>
@@ -36670,7 +36668,7 @@
         <v>251</v>
       </c>
       <c r="B252" s="119" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C252" s="116" t="s">
         <v>568</v>
@@ -36693,7 +36691,7 @@
         <v>252</v>
       </c>
       <c r="B253" s="119" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C253" s="116" t="s">
         <v>567</v>
@@ -36716,7 +36714,7 @@
         <v>253</v>
       </c>
       <c r="B254" s="119" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C254" s="116" t="s">
         <v>568</v>
@@ -36739,13 +36737,13 @@
         <v>254</v>
       </c>
       <c r="B255" s="119" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C255" s="116" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D255" s="138" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="E255" s="114">
         <v>1</v>
@@ -36762,13 +36760,13 @@
         <v>255</v>
       </c>
       <c r="B256" s="119" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C256" s="116" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D256" s="138" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E256" s="114">
         <v>2</v>
@@ -36785,13 +36783,13 @@
         <v>256</v>
       </c>
       <c r="B257" s="119" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C257" s="116" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D257" s="138" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E257" s="114">
         <v>3</v>
@@ -36808,13 +36806,13 @@
         <v>257</v>
       </c>
       <c r="B258" s="119" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C258" s="116" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D258" s="138" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E258" s="114">
         <v>4</v>
@@ -36831,13 +36829,13 @@
         <v>258</v>
       </c>
       <c r="B259" s="119" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C259" s="116" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D259" s="138" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E259" s="117">
         <v>5</v>
@@ -36854,13 +36852,13 @@
         <v>259</v>
       </c>
       <c r="B260" s="119" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C260" s="116" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D260" s="138" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E260" s="117">
         <v>6</v>
@@ -36877,13 +36875,13 @@
         <v>260</v>
       </c>
       <c r="B261" s="119" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C261" s="178" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="D261" s="174" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="E261" s="117">
         <v>7</v>
@@ -36900,13 +36898,13 @@
         <v>261</v>
       </c>
       <c r="B262" s="119" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C262" s="144" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D262" s="138" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E262" s="114">
         <v>99</v>
@@ -36974,10 +36972,10 @@
         <v>413</v>
       </c>
       <c r="C265" s="144" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D265" s="139" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E265" s="117">
         <v>99</v>
@@ -36996,7 +36994,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="121" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C266" s="116" t="s">
         <v>567</v>
@@ -37019,7 +37017,7 @@
         <v>266</v>
       </c>
       <c r="B267" s="121" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C267" s="116" t="s">
         <v>568</v>
@@ -37042,13 +37040,13 @@
         <v>267</v>
       </c>
       <c r="B268" s="121" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C268" s="144" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D268" s="138" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E268" s="117">
         <v>99</v>
@@ -37065,7 +37063,7 @@
         <v>268</v>
       </c>
       <c r="B269" s="121" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C269" s="116" t="s">
         <v>567</v>
@@ -37088,7 +37086,7 @@
         <v>269</v>
       </c>
       <c r="B270" s="121" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C270" s="116" t="s">
         <v>568</v>
@@ -37111,13 +37109,13 @@
         <v>270</v>
       </c>
       <c r="B271" s="121" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C271" s="144" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D271" s="138" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E271" s="117">
         <v>99</v>
@@ -37134,13 +37132,13 @@
         <v>271</v>
       </c>
       <c r="B272" s="121" t="s">
+        <v>812</v>
+      </c>
+      <c r="C272" s="116" t="s">
         <v>814</v>
       </c>
-      <c r="C272" s="116" t="s">
-        <v>816</v>
-      </c>
       <c r="D272" s="138" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E272" s="117">
         <v>1</v>
@@ -37157,13 +37155,13 @@
         <v>272</v>
       </c>
       <c r="B273" s="121" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C273" s="116" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D273" s="224" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="E273" s="117">
         <v>2</v>
@@ -37180,13 +37178,13 @@
         <v>273</v>
       </c>
       <c r="B274" s="121" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C274" s="116" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="D274" s="224" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="E274" s="114">
         <v>3</v>
@@ -37203,13 +37201,13 @@
         <v>274</v>
       </c>
       <c r="B275" s="121" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C275" s="116" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D275" s="138" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E275" s="114">
         <v>4</v>
@@ -37229,10 +37227,10 @@
         <v>437</v>
       </c>
       <c r="C276" s="116" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D276" s="138" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="E276" s="117">
         <v>1</v>
@@ -37252,10 +37250,10 @@
         <v>437</v>
       </c>
       <c r="C277" s="116" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D277" s="138" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="E277" s="117">
         <v>2</v>
@@ -37275,10 +37273,10 @@
         <v>437</v>
       </c>
       <c r="C278" s="116" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D278" s="138" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E278" s="114">
         <v>3</v>
@@ -37298,10 +37296,10 @@
         <v>437</v>
       </c>
       <c r="C279" s="116" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D279" s="138" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="E279" s="114">
         <v>4</v>
@@ -37321,16 +37319,16 @@
         <v>437</v>
       </c>
       <c r="C280" s="116" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D280" s="138" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E280" s="114">
         <v>77</v>
       </c>
       <c r="F280" s="55" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="G280" s="61"/>
       <c r="H280" s="111" t="str">
@@ -37346,10 +37344,10 @@
         <v>437</v>
       </c>
       <c r="C281" s="144" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D281" s="138" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E281" s="117">
         <v>99</v>
@@ -37366,7 +37364,7 @@
         <v>281</v>
       </c>
       <c r="B282" s="121" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C282" s="116" t="s">
         <v>567</v>
@@ -37389,7 +37387,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="121" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C283" s="116" t="s">
         <v>568</v>
@@ -37401,7 +37399,7 @@
         <v>2</v>
       </c>
       <c r="F283" s="118" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="G283" s="61"/>
       <c r="H283" s="111" t="str">
@@ -37414,13 +37412,13 @@
         <v>283</v>
       </c>
       <c r="B284" s="121" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C284" s="116" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="D284" s="138" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="E284" s="117">
         <v>1</v>
@@ -37437,13 +37435,13 @@
         <v>284</v>
       </c>
       <c r="B285" s="121" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C285" s="116" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D285" s="227" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="E285" s="117">
         <v>2</v>
@@ -37460,13 +37458,13 @@
         <v>285</v>
       </c>
       <c r="B286" s="121" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C286" s="116" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D286" s="138" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="E286" s="117">
         <v>3</v>
@@ -37483,19 +37481,19 @@
         <v>286</v>
       </c>
       <c r="B287" s="121" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C287" s="116" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D287" s="138" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E287" s="114">
         <v>77</v>
       </c>
       <c r="F287" s="121" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="G287" s="61"/>
       <c r="H287" s="111" t="str">

</xml_diff>